<commit_message>
add one basis character
</commit_message>
<xml_diff>
--- a/output/basis_character_new.xlsx
+++ b/output/basis_character_new.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3679" uniqueCount="2813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3680" uniqueCount="2814">
   <si>
     <t>Case4(2.11개)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -22529,12 +22529,16 @@
     <t>ㅍ</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>뾆</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -22654,7 +22658,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -22688,6 +22692,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4BACC6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -23134,7 +23144,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -23465,6 +23475,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -23757,9 +23770,9 @@
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" s="109" t="s">
         <v>82</v>
       </c>
@@ -23791,10 +23804,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="109"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="109"/>
       <c r="B3" s="17" t="s">
         <v>92</v>
@@ -23836,7 +23849,7 @@
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="109"/>
       <c r="B4" s="10"/>
       <c r="C4" s="20"/>
@@ -23857,7 +23870,7 @@
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="109"/>
       <c r="B5" s="17" t="s">
         <v>102</v>
@@ -23899,7 +23912,7 @@
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="109"/>
       <c r="B6" s="10"/>
       <c r="C6" s="20"/>
@@ -23920,7 +23933,7 @@
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="109"/>
       <c r="B7" s="17" t="s">
         <v>110</v>
@@ -23962,7 +23975,7 @@
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="109"/>
       <c r="B8" s="10"/>
       <c r="C8" s="20"/>
@@ -23983,7 +23996,7 @@
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="109"/>
       <c r="B9" s="17" t="s">
         <v>118</v>
@@ -24025,7 +24038,7 @@
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="109"/>
       <c r="B10" s="10"/>
       <c r="C10" s="20"/>
@@ -24046,7 +24059,7 @@
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" s="109"/>
       <c r="B11" s="17" t="s">
         <v>126</v>
@@ -24088,7 +24101,7 @@
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" s="109"/>
       <c r="B12" s="10"/>
       <c r="C12" s="20"/>
@@ -24109,7 +24122,7 @@
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13" s="109"/>
       <c r="B13" s="17" t="s">
         <v>132</v>
@@ -24151,7 +24164,7 @@
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14" s="109"/>
       <c r="B14" s="10"/>
       <c r="C14" s="20"/>
@@ -24172,7 +24185,7 @@
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" s="109"/>
       <c r="B15" s="19" t="s">
         <v>140</v>
@@ -24214,7 +24227,7 @@
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" s="109"/>
       <c r="B16" s="10"/>
       <c r="C16" s="20"/>
@@ -24235,7 +24248,7 @@
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17" s="109"/>
       <c r="B17" s="17" t="s">
         <v>148</v>
@@ -24277,7 +24290,7 @@
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" s="109"/>
       <c r="B18" s="10"/>
       <c r="C18" s="20"/>
@@ -24298,7 +24311,7 @@
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19" s="109"/>
       <c r="B19" s="17" t="s">
         <v>156</v>
@@ -24340,7 +24353,7 @@
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20" s="109"/>
       <c r="B20" s="10"/>
       <c r="C20" s="20"/>
@@ -24361,7 +24374,7 @@
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21" s="109"/>
       <c r="B21" s="17" t="s">
         <v>163</v>
@@ -24403,7 +24416,7 @@
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" s="109"/>
       <c r="B22" s="10"/>
       <c r="C22" s="20"/>
@@ -24424,7 +24437,7 @@
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" s="109"/>
       <c r="B23" s="19" t="s">
         <v>172</v>
@@ -24466,7 +24479,7 @@
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20">
       <c r="A24" s="109"/>
       <c r="B24" s="10"/>
       <c r="C24" s="20"/>
@@ -24487,7 +24500,7 @@
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20">
       <c r="A25" s="109"/>
       <c r="B25" s="17" t="s">
         <v>177</v>
@@ -24529,7 +24542,7 @@
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20">
       <c r="A26" s="109"/>
       <c r="B26" s="10"/>
       <c r="C26" s="20"/>
@@ -24550,7 +24563,7 @@
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20">
       <c r="A27" s="109"/>
       <c r="B27" s="19" t="s">
         <v>186</v>
@@ -24592,7 +24605,7 @@
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20">
       <c r="A28" s="109"/>
       <c r="B28" s="10"/>
       <c r="C28" s="20"/>
@@ -24613,7 +24626,7 @@
       <c r="S28" s="10"/>
       <c r="T28" s="10"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20">
       <c r="A29" s="109"/>
       <c r="B29" s="17" t="s">
         <v>195</v>
@@ -24655,7 +24668,7 @@
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20">
       <c r="A30" s="109"/>
       <c r="B30" s="10"/>
       <c r="C30" s="20"/>
@@ -24676,7 +24689,7 @@
       <c r="S30" s="10"/>
       <c r="T30" s="10"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20">
       <c r="A31" s="109"/>
       <c r="B31" s="17" t="s">
         <v>202</v>
@@ -24718,7 +24731,7 @@
       <c r="S31" s="10"/>
       <c r="T31" s="10"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20">
       <c r="A32" s="109"/>
       <c r="B32" s="10"/>
       <c r="C32" s="20"/>
@@ -24739,7 +24752,7 @@
       <c r="S32" s="10"/>
       <c r="T32" s="10"/>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41">
       <c r="A33" s="109"/>
       <c r="B33" s="17" t="s">
         <v>210</v>
@@ -24781,7 +24794,7 @@
       <c r="S33" s="10"/>
       <c r="T33" s="10"/>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41">
       <c r="A34" s="109"/>
       <c r="B34" s="10"/>
       <c r="C34" s="20"/>
@@ -24802,7 +24815,7 @@
       <c r="S34" s="10"/>
       <c r="T34" s="10"/>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41">
       <c r="A35" s="109"/>
       <c r="B35" s="17" t="s">
         <v>218</v>
@@ -24844,7 +24857,7 @@
       <c r="S35" s="10"/>
       <c r="T35" s="10"/>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41">
       <c r="A36" s="109"/>
       <c r="B36" s="10"/>
       <c r="C36" s="20"/>
@@ -24865,7 +24878,7 @@
       <c r="S36" s="10"/>
       <c r="T36" s="10"/>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41">
       <c r="A37" s="109"/>
       <c r="B37" s="17" t="s">
         <v>226</v>
@@ -24907,7 +24920,7 @@
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41">
       <c r="A38" s="109"/>
       <c r="B38" s="10"/>
       <c r="C38" s="20"/>
@@ -24928,7 +24941,7 @@
       <c r="S38" s="10"/>
       <c r="T38" s="10"/>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41">
       <c r="A39" s="109"/>
       <c r="B39" s="17" t="s">
         <v>234</v>
@@ -24970,7 +24983,7 @@
       <c r="S39" s="10"/>
       <c r="T39" s="10"/>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41">
       <c r="A40" s="109"/>
       <c r="B40" s="10"/>
       <c r="C40" s="20"/>
@@ -24982,7 +24995,7 @@
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41">
       <c r="B41" t="s">
         <v>242</v>
       </c>
@@ -25104,12 +25117,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41">
       <c r="A42" s="109" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41">
       <c r="A43" s="109"/>
       <c r="B43" t="s">
         <v>244</v>
@@ -25127,10 +25140,10 @@
         <v>248</v>
       </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41">
       <c r="A44" s="109"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41">
       <c r="A45" s="109"/>
       <c r="B45" s="17" t="s">
         <v>249</v>
@@ -25175,7 +25188,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41">
       <c r="A46" s="109"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -25183,7 +25196,7 @@
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41">
       <c r="A47" s="109"/>
       <c r="B47" s="17" t="s">
         <v>254</v>
@@ -25228,7 +25241,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41">
       <c r="A48" s="109"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -25236,7 +25249,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15">
       <c r="A49" s="109"/>
       <c r="B49" s="19" t="s">
         <v>259</v>
@@ -25281,7 +25294,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15">
       <c r="A50" s="109"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -25289,7 +25302,7 @@
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15">
       <c r="A51" s="109"/>
       <c r="B51" s="17" t="s">
         <v>264</v>
@@ -25334,7 +25347,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15">
       <c r="A52" s="109"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -25342,7 +25355,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15">
       <c r="A53" s="109"/>
       <c r="B53" s="19" t="s">
         <v>269</v>
@@ -25381,7 +25394,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15">
       <c r="A54" s="109"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -25389,7 +25402,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15">
       <c r="A55" s="109"/>
       <c r="B55" s="17" t="s">
         <v>272</v>
@@ -25434,7 +25447,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15">
       <c r="A56" s="109"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -25442,7 +25455,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15">
       <c r="A57" s="109"/>
       <c r="B57" s="17" t="s">
         <v>277</v>
@@ -25487,7 +25500,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15">
       <c r="A58" s="109"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -25495,7 +25508,7 @@
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15">
       <c r="A59" s="109"/>
       <c r="B59" s="17" t="s">
         <v>282</v>
@@ -25540,7 +25553,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15">
       <c r="A60" s="109"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
@@ -25548,7 +25561,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15">
       <c r="A61" s="109"/>
       <c r="B61" s="19" t="s">
         <v>287</v>
@@ -25593,7 +25606,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15">
       <c r="A62" s="109"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -25601,7 +25614,7 @@
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15">
       <c r="A63" s="109"/>
       <c r="B63" s="17" t="s">
         <v>292</v>
@@ -25646,7 +25659,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15">
       <c r="A64" s="109"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -25654,7 +25667,7 @@
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15">
       <c r="A65" s="109"/>
       <c r="B65" s="17" t="s">
         <v>297</v>
@@ -25696,7 +25709,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15">
       <c r="A66" s="109"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -25704,7 +25717,7 @@
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15">
       <c r="A67" s="109"/>
       <c r="B67" s="17" t="s">
         <v>301</v>
@@ -25749,7 +25762,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15">
       <c r="A68" s="109"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -25757,7 +25770,7 @@
       <c r="E68" s="10"/>
       <c r="F68" s="10"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15">
       <c r="A69" s="109"/>
       <c r="B69" s="17" t="s">
         <v>306</v>
@@ -25802,7 +25815,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15">
       <c r="A70" s="109"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -25810,7 +25823,7 @@
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15">
       <c r="A71" s="109"/>
       <c r="B71" s="17" t="s">
         <v>311</v>
@@ -25852,7 +25865,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15">
       <c r="A72" s="109"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -25860,7 +25873,7 @@
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15">
       <c r="A73" s="109"/>
       <c r="B73" s="17" t="s">
         <v>315</v>
@@ -25905,7 +25918,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15">
       <c r="A74" s="109"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -25913,7 +25926,7 @@
       <c r="E74" s="10"/>
       <c r="F74" s="10"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15">
       <c r="A75" s="109"/>
       <c r="B75" s="19" t="s">
         <v>320</v>
@@ -25958,7 +25971,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15">
       <c r="A76" s="109"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
@@ -25966,7 +25979,7 @@
       <c r="E76" s="10"/>
       <c r="F76" s="10"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15">
       <c r="A77" s="109"/>
       <c r="B77" s="17" t="s">
         <v>325</v>
@@ -26011,7 +26024,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15">
       <c r="A78" s="109"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
@@ -26019,7 +26032,7 @@
       <c r="E78" s="10"/>
       <c r="F78" s="10"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15">
       <c r="A79" s="109"/>
       <c r="B79" s="17" t="s">
         <v>330</v>
@@ -26064,7 +26077,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15">
       <c r="A80" s="109"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
@@ -26072,7 +26085,7 @@
       <c r="E80" s="10"/>
       <c r="F80" s="10"/>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:41">
       <c r="A81" s="109"/>
       <c r="B81" s="17" t="s">
         <v>335</v>
@@ -26117,7 +26130,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:41">
       <c r="A82" s="109"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
@@ -26125,7 +26138,7 @@
       <c r="E82" s="10"/>
       <c r="F82" s="10"/>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:41">
       <c r="B83" t="s">
         <v>242</v>
       </c>
@@ -26247,12 +26260,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:41">
       <c r="A84" s="109" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:41">
       <c r="A85" s="109"/>
       <c r="B85" t="s">
         <v>341</v>
@@ -26276,10 +26289,10 @@
         <v>347</v>
       </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:41">
       <c r="A86" s="109"/>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:41">
       <c r="A87" s="109"/>
       <c r="B87" s="17" t="s">
         <v>348</v>
@@ -26330,7 +26343,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:41">
       <c r="A88" s="109"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -26340,7 +26353,7 @@
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:41">
       <c r="A89" s="109"/>
       <c r="B89" s="17" t="s">
         <v>355</v>
@@ -26388,7 +26401,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:41">
       <c r="A90" s="109"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
@@ -26398,7 +26411,7 @@
       <c r="G90" s="10"/>
       <c r="H90" s="10"/>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:41">
       <c r="A91" s="109"/>
       <c r="B91" s="17" t="s">
         <v>361</v>
@@ -26446,7 +26459,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:41">
       <c r="A92" s="109"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
@@ -26456,7 +26469,7 @@
       <c r="G92" s="10"/>
       <c r="H92" s="10"/>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:41">
       <c r="A93" s="109"/>
       <c r="B93" s="19" t="s">
         <v>367</v>
@@ -26507,7 +26520,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:41">
       <c r="A94" s="109"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -26517,7 +26530,7 @@
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:41">
       <c r="A95" s="109"/>
       <c r="B95" s="19" t="s">
         <v>374</v>
@@ -26565,7 +26578,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:41">
       <c r="A96" s="109"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
@@ -26575,7 +26588,7 @@
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17">
       <c r="A97" s="109"/>
       <c r="B97" s="17" t="s">
         <v>380</v>
@@ -26620,7 +26633,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17">
       <c r="A98" s="109"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -26630,7 +26643,7 @@
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17">
       <c r="A99" s="109"/>
       <c r="B99" s="17" t="s">
         <v>385</v>
@@ -26675,7 +26688,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17">
       <c r="A100" s="109"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
@@ -26685,7 +26698,7 @@
       <c r="G100" s="10"/>
       <c r="H100" s="10"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17">
       <c r="A101" s="109"/>
       <c r="B101" s="17" t="s">
         <v>390</v>
@@ -26733,7 +26746,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17">
       <c r="A102" s="109"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
@@ -26743,7 +26756,7 @@
       <c r="G102" s="10"/>
       <c r="H102" s="10"/>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17">
       <c r="A103" s="109"/>
       <c r="B103" s="17" t="s">
         <v>101</v>
@@ -26776,7 +26789,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17">
       <c r="A104" s="109"/>
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
@@ -26786,7 +26799,7 @@
       <c r="G104" s="10"/>
       <c r="H104" s="10"/>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17">
       <c r="A105" s="109"/>
       <c r="B105" s="17" t="s">
         <v>397</v>
@@ -26834,7 +26847,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17">
       <c r="A106" s="109"/>
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
@@ -26844,7 +26857,7 @@
       <c r="G106" s="10"/>
       <c r="H106" s="10"/>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17">
       <c r="A107" s="109"/>
       <c r="B107" s="17" t="s">
         <v>403</v>
@@ -26895,7 +26908,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17">
       <c r="A108" s="109"/>
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
@@ -26905,7 +26918,7 @@
       <c r="G108" s="10"/>
       <c r="H108" s="10"/>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17">
       <c r="A109" s="109"/>
       <c r="B109" s="17" t="s">
         <v>410</v>
@@ -26956,7 +26969,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17">
       <c r="A110" s="109"/>
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
@@ -26966,7 +26979,7 @@
       <c r="G110" s="10"/>
       <c r="H110" s="10"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17">
       <c r="A111" s="109"/>
       <c r="B111" s="17" t="s">
         <v>417</v>
@@ -27014,7 +27027,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17">
       <c r="A112" s="109"/>
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
@@ -27024,7 +27037,7 @@
       <c r="G112" s="10"/>
       <c r="H112" s="10"/>
     </row>
-    <row r="113" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:99">
       <c r="A113" s="109"/>
       <c r="B113" s="17" t="s">
         <v>423</v>
@@ -27069,7 +27082,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="114" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:99">
       <c r="A114" s="109"/>
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
@@ -27079,7 +27092,7 @@
       <c r="G114" s="10"/>
       <c r="H114" s="10"/>
     </row>
-    <row r="115" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:99">
       <c r="A115" s="109"/>
       <c r="B115" s="17" t="s">
         <v>428</v>
@@ -27124,7 +27137,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="116" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:99">
       <c r="A116" s="109"/>
       <c r="B116" s="10"/>
       <c r="C116" s="10"/>
@@ -27134,7 +27147,7 @@
       <c r="G116" s="10"/>
       <c r="H116" s="10"/>
     </row>
-    <row r="117" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:99">
       <c r="A117" s="109"/>
       <c r="B117" s="17" t="s">
         <v>433</v>
@@ -27182,7 +27195,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="118" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:99">
       <c r="A118" s="109"/>
       <c r="B118" s="10"/>
       <c r="C118" s="10"/>
@@ -27192,7 +27205,7 @@
       <c r="G118" s="10"/>
       <c r="H118" s="10"/>
     </row>
-    <row r="119" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:99">
       <c r="A119" s="109"/>
       <c r="B119" s="17" t="s">
         <v>439</v>
@@ -27243,7 +27256,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="120" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:99">
       <c r="A120" s="109"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
@@ -27253,7 +27266,7 @@
       <c r="G120" s="10"/>
       <c r="H120" s="10"/>
     </row>
-    <row r="121" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:99">
       <c r="A121" s="109"/>
       <c r="B121" s="19" t="s">
         <v>446</v>
@@ -27295,7 +27308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="122" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:99">
       <c r="A122" s="109"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
@@ -27305,7 +27318,7 @@
       <c r="G122" s="10"/>
       <c r="H122" s="10"/>
     </row>
-    <row r="123" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:99">
       <c r="A123" s="109"/>
       <c r="B123" s="17" t="s">
         <v>450</v>
@@ -27356,7 +27369,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="124" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:99">
       <c r="A124" s="109"/>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
@@ -27366,7 +27379,7 @@
       <c r="G124" s="10"/>
       <c r="H124" s="10"/>
     </row>
-    <row r="125" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:99">
       <c r="A125" s="25"/>
       <c r="B125" t="s">
         <v>242</v>
@@ -27489,7 +27502,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:99">
       <c r="A126" s="108" t="s">
         <v>457</v>
       </c>
@@ -27592,7 +27605,7 @@
       <c r="CT126" s="10"/>
       <c r="CU126" s="10"/>
     </row>
-    <row r="127" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:99">
       <c r="A127" s="108"/>
       <c r="B127" s="10" t="s">
         <v>83</v>
@@ -27711,7 +27724,7 @@
       <c r="CT127" s="10"/>
       <c r="CU127" s="10"/>
     </row>
-    <row r="128" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:99">
       <c r="A128" s="108"/>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
@@ -27812,7 +27825,7 @@
       <c r="CT128" s="10"/>
       <c r="CU128" s="10"/>
     </row>
-    <row r="129" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:99">
       <c r="A129" s="108"/>
       <c r="B129" s="18" t="s">
         <v>458</v>
@@ -28071,7 +28084,7 @@
       <c r="CT129" s="10"/>
       <c r="CU129" s="10"/>
     </row>
-    <row r="130" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:99">
       <c r="A130" s="108"/>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
@@ -28172,7 +28185,7 @@
       <c r="CT130" s="10"/>
       <c r="CU130" s="10"/>
     </row>
-    <row r="131" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:99">
       <c r="A131" s="108"/>
       <c r="B131" s="17" t="s">
         <v>537</v>
@@ -28367,7 +28380,7 @@
       <c r="CT131" s="10"/>
       <c r="CU131" s="10"/>
     </row>
-    <row r="132" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:99">
       <c r="A132" s="108"/>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
@@ -28468,7 +28481,7 @@
       <c r="CT132" s="10"/>
       <c r="CU132" s="10"/>
     </row>
-    <row r="133" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:99">
       <c r="A133" s="108"/>
       <c r="B133" s="17" t="s">
         <v>584</v>
@@ -28703,7 +28716,7 @@
       <c r="CT133" s="10"/>
       <c r="CU133" s="10"/>
     </row>
-    <row r="134" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:99">
       <c r="A134" s="108"/>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
@@ -28804,7 +28817,7 @@
       <c r="CT134" s="10"/>
       <c r="CU134" s="10"/>
     </row>
-    <row r="135" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:99">
       <c r="A135" s="108"/>
       <c r="B135" s="17" t="s">
         <v>651</v>
@@ -29027,7 +29040,7 @@
       <c r="CT135" s="10"/>
       <c r="CU135" s="10"/>
     </row>
-    <row r="136" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:99">
       <c r="A136" s="108"/>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
@@ -29128,7 +29141,7 @@
       <c r="CT136" s="10"/>
       <c r="CU136" s="10"/>
     </row>
-    <row r="137" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:99">
       <c r="A137" s="108"/>
       <c r="B137" s="17" t="s">
         <v>712</v>
@@ -29315,7 +29328,7 @@
       <c r="CT137" s="10"/>
       <c r="CU137" s="10"/>
     </row>
-    <row r="138" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:99">
       <c r="A138" s="108"/>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -29416,7 +29429,7 @@
       <c r="CT138" s="10"/>
       <c r="CU138" s="10"/>
     </row>
-    <row r="139" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:99">
       <c r="A139" s="108"/>
       <c r="B139" s="17" t="s">
         <v>755</v>
@@ -29631,7 +29644,7 @@
       <c r="CT139" s="10"/>
       <c r="CU139" s="10"/>
     </row>
-    <row r="140" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:99">
       <c r="A140" s="108"/>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -29732,7 +29745,7 @@
       <c r="CT140" s="10"/>
       <c r="CU140" s="10"/>
     </row>
-    <row r="141" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:99">
       <c r="A141" s="108"/>
       <c r="B141" s="17" t="s">
         <v>812</v>
@@ -29959,7 +29972,7 @@
       <c r="CT141" s="10"/>
       <c r="CU141" s="10"/>
     </row>
-    <row r="142" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:99">
       <c r="A142" s="108"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -30060,7 +30073,7 @@
       <c r="CT142" s="10"/>
       <c r="CU142" s="10"/>
     </row>
-    <row r="143" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:99">
       <c r="A143" s="108"/>
       <c r="B143" s="18" t="s">
         <v>875</v>
@@ -30289,7 +30302,7 @@
       <c r="CT143" s="10"/>
       <c r="CU143" s="10"/>
     </row>
-    <row r="144" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:99">
       <c r="A144" s="108"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -30390,7 +30403,7 @@
       <c r="CT144" s="10"/>
       <c r="CU144" s="10"/>
     </row>
-    <row r="145" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:99">
       <c r="A145" s="108"/>
       <c r="B145" s="17" t="s">
         <v>939</v>
@@ -30575,7 +30588,7 @@
       <c r="CT145" s="10"/>
       <c r="CU145" s="10"/>
     </row>
-    <row r="146" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:99">
       <c r="A146" s="108"/>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -30676,7 +30689,7 @@
       <c r="CT146" s="10"/>
       <c r="CU146" s="10"/>
     </row>
-    <row r="147" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:99">
       <c r="A147" s="108"/>
       <c r="B147" s="17" t="s">
         <v>981</v>
@@ -30927,7 +30940,7 @@
       <c r="CT147" s="10"/>
       <c r="CU147" s="10"/>
     </row>
-    <row r="148" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:99">
       <c r="A148" s="108"/>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
@@ -31028,7 +31041,7 @@
       <c r="CT148" s="10"/>
       <c r="CU148" s="10"/>
     </row>
-    <row r="149" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:99">
       <c r="A149" s="108"/>
       <c r="B149" s="17" t="s">
         <v>1055</v>
@@ -31199,7 +31212,7 @@
       <c r="CT149" s="10"/>
       <c r="CU149" s="10"/>
     </row>
-    <row r="150" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:99">
       <c r="A150" s="108"/>
       <c r="B150" s="10"/>
       <c r="C150" s="10"/>
@@ -31300,7 +31313,7 @@
       <c r="CT150" s="10"/>
       <c r="CU150" s="10"/>
     </row>
-    <row r="151" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:99">
       <c r="A151" s="108"/>
       <c r="B151" s="17" t="s">
         <v>1090</v>
@@ -31585,7 +31598,7 @@
       <c r="CT151" s="10"/>
       <c r="CU151" s="10"/>
     </row>
-    <row r="152" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:99">
       <c r="A152" s="108"/>
       <c r="B152" s="10"/>
       <c r="C152" s="10"/>
@@ -31686,7 +31699,7 @@
       <c r="CT152" s="10"/>
       <c r="CU152" s="10"/>
     </row>
-    <row r="153" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:99">
       <c r="A153" s="108"/>
       <c r="B153" s="17" t="s">
         <v>1182</v>
@@ -31911,7 +31924,7 @@
       <c r="CT153" s="10"/>
       <c r="CU153" s="10"/>
     </row>
-    <row r="154" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:99">
       <c r="A154" s="108"/>
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
@@ -32012,7 +32025,7 @@
       <c r="CT154" s="10"/>
       <c r="CU154" s="10"/>
     </row>
-    <row r="155" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:99">
       <c r="A155" s="108"/>
       <c r="B155" s="17" t="s">
         <v>1244</v>
@@ -32189,7 +32202,7 @@
       <c r="CT155" s="10"/>
       <c r="CU155" s="10"/>
     </row>
-    <row r="156" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:99">
       <c r="A156" s="108"/>
       <c r="B156" s="10"/>
       <c r="C156" s="10"/>
@@ -32290,7 +32303,7 @@
       <c r="CT156" s="10"/>
       <c r="CU156" s="10"/>
     </row>
-    <row r="157" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:99">
       <c r="A157" s="108"/>
       <c r="B157" s="18" t="s">
         <v>1282</v>
@@ -32493,7 +32506,7 @@
       <c r="CT157" s="10"/>
       <c r="CU157" s="10"/>
     </row>
-    <row r="158" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:99">
       <c r="A158" s="108"/>
       <c r="B158" s="10"/>
       <c r="C158" s="10"/>
@@ -32594,7 +32607,7 @@
       <c r="CT158" s="10"/>
       <c r="CU158" s="10"/>
     </row>
-    <row r="159" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:99">
       <c r="A159" s="108"/>
       <c r="B159" s="17" t="s">
         <v>1333</v>
@@ -32789,7 +32802,7 @@
       <c r="CT159" s="10"/>
       <c r="CU159" s="10"/>
     </row>
-    <row r="160" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:99">
       <c r="A160" s="108"/>
       <c r="B160" s="10"/>
       <c r="C160" s="10"/>
@@ -32890,7 +32903,7 @@
       <c r="CT160" s="10"/>
       <c r="CU160" s="10"/>
     </row>
-    <row r="161" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:99">
       <c r="A161" s="108"/>
       <c r="B161" s="17" t="s">
         <v>1380</v>
@@ -33079,7 +33092,7 @@
       <c r="CT161" s="10"/>
       <c r="CU161" s="10"/>
     </row>
-    <row r="162" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:99">
       <c r="A162" s="108"/>
       <c r="B162" s="10"/>
       <c r="C162" s="10"/>
@@ -33180,7 +33193,7 @@
       <c r="CT162" s="10"/>
       <c r="CU162" s="10"/>
     </row>
-    <row r="163" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:99">
       <c r="A163" s="108"/>
       <c r="B163" s="17" t="s">
         <v>1424</v>
@@ -33383,7 +33396,7 @@
       <c r="CT163" s="10"/>
       <c r="CU163" s="10"/>
     </row>
-    <row r="164" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:99">
       <c r="A164" s="108"/>
       <c r="B164" s="10"/>
       <c r="C164" s="10"/>
@@ -33484,7 +33497,7 @@
       <c r="CT164" s="10"/>
       <c r="CU164" s="10"/>
     </row>
-    <row r="165" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:99">
       <c r="A165" s="108"/>
       <c r="B165" s="17" t="s">
         <v>1475</v>
@@ -33685,7 +33698,7 @@
       <c r="CT165" s="10"/>
       <c r="CU165" s="10"/>
     </row>
-    <row r="166" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:99">
       <c r="A166" s="108"/>
       <c r="B166" s="10"/>
       <c r="C166" s="10"/>
@@ -33786,7 +33799,7 @@
       <c r="CT166" s="10"/>
       <c r="CU166" s="10"/>
     </row>
-    <row r="167" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:99">
       <c r="A167" s="10"/>
       <c r="B167" s="10" t="s">
         <v>242</v>
@@ -33967,7 +33980,7 @@
       <c r="CT167" s="10"/>
       <c r="CU167" s="10"/>
     </row>
-    <row r="168" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:99">
       <c r="A168" s="108" t="s">
         <v>1525</v>
       </c>
@@ -34070,7 +34083,7 @@
       <c r="CT168" s="10"/>
       <c r="CU168" s="10"/>
     </row>
-    <row r="169" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:99">
       <c r="A169" s="108"/>
       <c r="B169" s="10" t="s">
         <v>244</v>
@@ -34181,7 +34194,7 @@
       <c r="CT169" s="10"/>
       <c r="CU169" s="10"/>
     </row>
-    <row r="170" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:99">
       <c r="A170" s="108"/>
       <c r="B170" s="10"/>
       <c r="C170" s="10"/>
@@ -34282,7 +34295,7 @@
       <c r="CT170" s="10"/>
       <c r="CU170" s="10"/>
     </row>
-    <row r="171" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:99">
       <c r="A171" s="108"/>
       <c r="B171" s="17" t="s">
         <v>1526</v>
@@ -34461,7 +34474,7 @@
       <c r="CT171" s="10"/>
       <c r="CU171" s="10"/>
     </row>
-    <row r="172" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:99">
       <c r="A172" s="108"/>
       <c r="B172" s="10"/>
       <c r="C172" s="10"/>
@@ -34562,7 +34575,7 @@
       <c r="CT172" s="10"/>
       <c r="CU172" s="10"/>
     </row>
-    <row r="173" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:99">
       <c r="A173" s="108"/>
       <c r="B173" s="17" t="s">
         <v>1565</v>
@@ -34723,7 +34736,7 @@
       <c r="CT173" s="10"/>
       <c r="CU173" s="10"/>
     </row>
-    <row r="174" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:99">
       <c r="A174" s="108"/>
       <c r="B174" s="10"/>
       <c r="C174" s="10"/>
@@ -34824,7 +34837,7 @@
       <c r="CT174" s="10"/>
       <c r="CU174" s="10"/>
     </row>
-    <row r="175" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:99">
       <c r="A175" s="108"/>
       <c r="B175" s="17" t="s">
         <v>1595</v>
@@ -35005,7 +35018,7 @@
       <c r="CT175" s="10"/>
       <c r="CU175" s="10"/>
     </row>
-    <row r="176" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:99">
       <c r="A176" s="108"/>
       <c r="B176" s="10"/>
       <c r="C176" s="10"/>
@@ -35106,7 +35119,7 @@
       <c r="CT176" s="10"/>
       <c r="CU176" s="10"/>
     </row>
-    <row r="177" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:99">
       <c r="A177" s="108"/>
       <c r="B177" s="17" t="s">
         <v>1635</v>
@@ -35271,7 +35284,7 @@
       <c r="CT177" s="10"/>
       <c r="CU177" s="10"/>
     </row>
-    <row r="178" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:99">
       <c r="A178" s="108"/>
       <c r="B178" s="10"/>
       <c r="C178" s="10"/>
@@ -35372,7 +35385,7 @@
       <c r="CT178" s="10"/>
       <c r="CU178" s="10"/>
     </row>
-    <row r="179" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:99">
       <c r="A179" s="108"/>
       <c r="B179" s="17" t="s">
         <v>1667</v>
@@ -35507,7 +35520,7 @@
       <c r="CT179" s="10"/>
       <c r="CU179" s="10"/>
     </row>
-    <row r="180" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:99">
       <c r="A180" s="108"/>
       <c r="B180" s="10"/>
       <c r="C180" s="10"/>
@@ -35608,7 +35621,7 @@
       <c r="CT180" s="10"/>
       <c r="CU180" s="10"/>
     </row>
-    <row r="181" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:99">
       <c r="A181" s="108"/>
       <c r="B181" s="18" t="s">
         <v>1684</v>
@@ -35781,7 +35794,7 @@
       <c r="CT181" s="10"/>
       <c r="CU181" s="10"/>
     </row>
-    <row r="182" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:99">
       <c r="A182" s="108"/>
       <c r="B182" s="10"/>
       <c r="C182" s="10"/>
@@ -35882,7 +35895,7 @@
       <c r="CT182" s="10"/>
       <c r="CU182" s="10"/>
     </row>
-    <row r="183" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:99">
       <c r="A183" s="108"/>
       <c r="B183" s="18" t="s">
         <v>1720</v>
@@ -36051,7 +36064,7 @@
       <c r="CT183" s="10"/>
       <c r="CU183" s="10"/>
     </row>
-    <row r="184" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:99">
       <c r="A184" s="108"/>
       <c r="B184" s="10"/>
       <c r="C184" s="10"/>
@@ -36152,7 +36165,7 @@
       <c r="CT184" s="10"/>
       <c r="CU184" s="10"/>
     </row>
-    <row r="185" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:99">
       <c r="A185" s="108"/>
       <c r="B185" s="17" t="s">
         <v>1754</v>
@@ -36317,7 +36330,7 @@
       <c r="CT185" s="10"/>
       <c r="CU185" s="10"/>
     </row>
-    <row r="186" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:99">
       <c r="A186" s="108"/>
       <c r="B186" s="10"/>
       <c r="C186" s="10"/>
@@ -36418,7 +36431,7 @@
       <c r="CT186" s="10"/>
       <c r="CU186" s="10"/>
     </row>
-    <row r="187" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:99">
       <c r="A187" s="108"/>
       <c r="B187" s="17" t="s">
         <v>1786</v>
@@ -36555,7 +36568,7 @@
       <c r="CT187" s="10"/>
       <c r="CU187" s="10"/>
     </row>
-    <row r="188" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:99">
       <c r="A188" s="108"/>
       <c r="B188" s="10"/>
       <c r="C188" s="10"/>
@@ -36656,7 +36669,7 @@
       <c r="CT188" s="10"/>
       <c r="CU188" s="10"/>
     </row>
-    <row r="189" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:99">
       <c r="A189" s="108"/>
       <c r="B189" s="17" t="s">
         <v>1804</v>
@@ -36839,7 +36852,7 @@
       <c r="CT189" s="10"/>
       <c r="CU189" s="10"/>
     </row>
-    <row r="190" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:99">
       <c r="A190" s="108"/>
       <c r="B190" s="10"/>
       <c r="C190" s="10"/>
@@ -36940,7 +36953,7 @@
       <c r="CT190" s="10"/>
       <c r="CU190" s="10"/>
     </row>
-    <row r="191" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:99">
       <c r="A191" s="108"/>
       <c r="B191" s="17" t="s">
         <v>1845</v>
@@ -37085,7 +37098,7 @@
       <c r="CT191" s="10"/>
       <c r="CU191" s="10"/>
     </row>
-    <row r="192" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:99">
       <c r="A192" s="108"/>
       <c r="B192" s="10"/>
       <c r="C192" s="10"/>
@@ -37186,7 +37199,7 @@
       <c r="CT192" s="10"/>
       <c r="CU192" s="10"/>
     </row>
-    <row r="193" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:99">
       <c r="A193" s="108"/>
       <c r="B193" s="17" t="s">
         <v>1867</v>
@@ -37387,7 +37400,7 @@
       <c r="CT193" s="10"/>
       <c r="CU193" s="10"/>
     </row>
-    <row r="194" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:99">
       <c r="A194" s="108"/>
       <c r="B194" s="10"/>
       <c r="C194" s="10"/>
@@ -37488,7 +37501,7 @@
       <c r="CT194" s="10"/>
       <c r="CU194" s="10"/>
     </row>
-    <row r="195" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:99">
       <c r="A195" s="108"/>
       <c r="B195" s="17" t="s">
         <v>1917</v>
@@ -37655,7 +37668,7 @@
       <c r="CT195" s="10"/>
       <c r="CU195" s="10"/>
     </row>
-    <row r="196" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:99">
       <c r="A196" s="108"/>
       <c r="B196" s="10"/>
       <c r="C196" s="10"/>
@@ -37756,7 +37769,7 @@
       <c r="CT196" s="10"/>
       <c r="CU196" s="10"/>
     </row>
-    <row r="197" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:99">
       <c r="A197" s="108"/>
       <c r="B197" s="17" t="s">
         <v>1950</v>
@@ -37893,7 +37906,7 @@
       <c r="CT197" s="10"/>
       <c r="CU197" s="10"/>
     </row>
-    <row r="198" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:99">
       <c r="A198" s="108"/>
       <c r="B198" s="10"/>
       <c r="C198" s="10"/>
@@ -37994,7 +38007,7 @@
       <c r="CT198" s="10"/>
       <c r="CU198" s="10"/>
     </row>
-    <row r="199" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:99">
       <c r="A199" s="108"/>
       <c r="B199" s="17" t="s">
         <v>1968</v>
@@ -38147,7 +38160,7 @@
       <c r="CT199" s="10"/>
       <c r="CU199" s="10"/>
     </row>
-    <row r="200" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:99">
       <c r="A200" s="108"/>
       <c r="B200" s="10"/>
       <c r="C200" s="10"/>
@@ -38248,7 +38261,7 @@
       <c r="CT200" s="10"/>
       <c r="CU200" s="10"/>
     </row>
-    <row r="201" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:99">
       <c r="A201" s="108"/>
       <c r="B201" s="17" t="s">
         <v>1994</v>
@@ -38395,7 +38408,7 @@
       <c r="CT201" s="10"/>
       <c r="CU201" s="10"/>
     </row>
-    <row r="202" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:99">
       <c r="A202" s="108"/>
       <c r="B202" s="10"/>
       <c r="C202" s="10"/>
@@ -38496,7 +38509,7 @@
       <c r="CT202" s="10"/>
       <c r="CU202" s="10"/>
     </row>
-    <row r="203" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:99">
       <c r="A203" s="108"/>
       <c r="B203" s="17" t="s">
         <v>2016</v>
@@ -38651,7 +38664,7 @@
       <c r="CT203" s="10"/>
       <c r="CU203" s="10"/>
     </row>
-    <row r="204" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:99">
       <c r="A204" s="108"/>
       <c r="B204" s="10"/>
       <c r="C204" s="10"/>
@@ -38751,7 +38764,7 @@
       <c r="CT204" s="10"/>
       <c r="CU204" s="10"/>
     </row>
-    <row r="205" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:99">
       <c r="A205" s="108"/>
       <c r="B205" s="17" t="s">
         <v>2043</v>
@@ -38912,7 +38925,7 @@
       <c r="CT205" s="10"/>
       <c r="CU205" s="10"/>
     </row>
-    <row r="206" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:99">
       <c r="A206" s="108"/>
       <c r="B206" s="10"/>
       <c r="C206" s="10"/>
@@ -39013,7 +39026,7 @@
       <c r="CT206" s="10"/>
       <c r="CU206" s="10"/>
     </row>
-    <row r="207" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:99">
       <c r="A207" s="108"/>
       <c r="B207" s="17" t="s">
         <v>2073</v>
@@ -39188,7 +39201,7 @@
       <c r="CT207" s="10"/>
       <c r="CU207" s="10"/>
     </row>
-    <row r="208" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:99">
       <c r="A208" s="108"/>
       <c r="B208" s="10"/>
       <c r="C208" s="10"/>
@@ -39289,7 +39302,7 @@
       <c r="CT208" s="10"/>
       <c r="CU208" s="10"/>
     </row>
-    <row r="209" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:99">
       <c r="A209" s="10"/>
       <c r="B209" s="10" t="s">
         <v>242</v>
@@ -39470,7 +39483,7 @@
       <c r="CT209" s="10"/>
       <c r="CU209" s="10"/>
     </row>
-    <row r="210" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:99">
       <c r="A210" s="108" t="s">
         <v>2110</v>
       </c>
@@ -39573,7 +39586,7 @@
       <c r="CT210" s="10"/>
       <c r="CU210" s="10"/>
     </row>
-    <row r="211" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:99">
       <c r="A211" s="108"/>
       <c r="B211" s="10" t="s">
         <v>341</v>
@@ -39688,7 +39701,7 @@
       <c r="CT211" s="10"/>
       <c r="CU211" s="10"/>
     </row>
-    <row r="212" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:99">
       <c r="A212" s="108"/>
       <c r="B212" s="10"/>
       <c r="C212" s="10"/>
@@ -39789,7 +39802,7 @@
       <c r="CT212" s="10"/>
       <c r="CU212" s="10"/>
     </row>
-    <row r="213" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:99">
       <c r="A213" s="108"/>
       <c r="B213" s="17" t="s">
         <v>2111</v>
@@ -39954,7 +39967,7 @@
       <c r="CT213" s="10"/>
       <c r="CU213" s="10"/>
     </row>
-    <row r="214" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:99">
       <c r="A214" s="108"/>
       <c r="B214" s="10"/>
       <c r="C214" s="10"/>
@@ -40055,7 +40068,7 @@
       <c r="CT214" s="10"/>
       <c r="CU214" s="10"/>
     </row>
-    <row r="215" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:99">
       <c r="A215" s="108"/>
       <c r="B215" s="17" t="s">
         <v>2143</v>
@@ -40204,7 +40217,7 @@
       <c r="CT215" s="10"/>
       <c r="CU215" s="10"/>
     </row>
-    <row r="216" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:99">
       <c r="A216" s="108"/>
       <c r="B216" s="10"/>
       <c r="C216" s="10"/>
@@ -40305,7 +40318,7 @@
       <c r="CT216" s="10"/>
       <c r="CU216" s="10"/>
     </row>
-    <row r="217" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:99">
       <c r="A217" s="108"/>
       <c r="B217" s="17" t="s">
         <v>2167</v>
@@ -40436,7 +40449,7 @@
       <c r="CT217" s="10"/>
       <c r="CU217" s="10"/>
     </row>
-    <row r="218" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:99">
       <c r="A218" s="108"/>
       <c r="B218" s="10"/>
       <c r="C218" s="10"/>
@@ -40537,7 +40550,7 @@
       <c r="CT218" s="10"/>
       <c r="CU218" s="10"/>
     </row>
-    <row r="219" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:99">
       <c r="A219" s="108"/>
       <c r="B219" s="17" t="s">
         <v>2182</v>
@@ -40668,7 +40681,7 @@
       <c r="CT219" s="10"/>
       <c r="CU219" s="10"/>
     </row>
-    <row r="220" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:99">
       <c r="A220" s="108"/>
       <c r="B220" s="10"/>
       <c r="C220" s="10"/>
@@ -40769,7 +40782,7 @@
       <c r="CT220" s="10"/>
       <c r="CU220" s="10"/>
     </row>
-    <row r="221" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:99">
       <c r="A221" s="108"/>
       <c r="B221" s="17" t="s">
         <v>2197</v>
@@ -40892,7 +40905,7 @@
       <c r="CT221" s="10"/>
       <c r="CU221" s="10"/>
     </row>
-    <row r="222" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:99">
       <c r="A222" s="108"/>
       <c r="B222" s="10"/>
       <c r="C222" s="10"/>
@@ -40993,7 +41006,7 @@
       <c r="CT222" s="10"/>
       <c r="CU222" s="10"/>
     </row>
-    <row r="223" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:99">
       <c r="A223" s="108"/>
       <c r="B223" s="17" t="s">
         <v>2208</v>
@@ -41126,7 +41139,7 @@
       <c r="CT223" s="10"/>
       <c r="CU223" s="10"/>
     </row>
-    <row r="224" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:99">
       <c r="A224" s="108"/>
       <c r="B224" s="10"/>
       <c r="C224" s="10"/>
@@ -41227,7 +41240,7 @@
       <c r="CT224" s="10"/>
       <c r="CU224" s="10"/>
     </row>
-    <row r="225" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:99">
       <c r="A225" s="108"/>
       <c r="B225" s="17" t="s">
         <v>2224</v>
@@ -41356,7 +41369,7 @@
       <c r="CT225" s="10"/>
       <c r="CU225" s="10"/>
     </row>
-    <row r="226" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:99">
       <c r="A226" s="108"/>
       <c r="B226" s="10"/>
       <c r="C226" s="10"/>
@@ -41457,7 +41470,7 @@
       <c r="CT226" s="10"/>
       <c r="CU226" s="10"/>
     </row>
-    <row r="227" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:99">
       <c r="A227" s="108"/>
       <c r="B227" s="17" t="s">
         <v>2238</v>
@@ -41586,7 +41599,7 @@
       <c r="CT227" s="10"/>
       <c r="CU227" s="10"/>
     </row>
-    <row r="228" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:99">
       <c r="A228" s="108"/>
       <c r="B228" s="10"/>
       <c r="C228" s="10"/>
@@ -41687,7 +41700,7 @@
       <c r="CT228" s="10"/>
       <c r="CU228" s="10"/>
     </row>
-    <row r="229" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:99">
       <c r="A229" s="108"/>
       <c r="B229" s="10"/>
       <c r="C229" s="10"/>
@@ -41788,7 +41801,7 @@
       <c r="CT229" s="10"/>
       <c r="CU229" s="10"/>
     </row>
-    <row r="230" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:99">
       <c r="A230" s="108"/>
       <c r="B230" s="10"/>
       <c r="C230" s="10"/>
@@ -41889,7 +41902,7 @@
       <c r="CT230" s="10"/>
       <c r="CU230" s="10"/>
     </row>
-    <row r="231" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:99">
       <c r="A231" s="108"/>
       <c r="B231" s="17" t="s">
         <v>2252</v>
@@ -42044,7 +42057,7 @@
       <c r="CT231" s="10"/>
       <c r="CU231" s="10"/>
     </row>
-    <row r="232" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:99">
       <c r="A232" s="108"/>
       <c r="B232" s="10"/>
       <c r="C232" s="10"/>
@@ -42145,7 +42158,7 @@
       <c r="CT232" s="10"/>
       <c r="CU232" s="10"/>
     </row>
-    <row r="233" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:99">
       <c r="A233" s="108"/>
       <c r="B233" s="17" t="s">
         <v>2279</v>
@@ -42272,7 +42285,7 @@
       <c r="CT233" s="10"/>
       <c r="CU233" s="10"/>
     </row>
-    <row r="234" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:99">
       <c r="A234" s="108"/>
       <c r="B234" s="10"/>
       <c r="C234" s="10"/>
@@ -42373,7 +42386,7 @@
       <c r="CT234" s="10"/>
       <c r="CU234" s="10"/>
     </row>
-    <row r="235" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:99">
       <c r="A235" s="108"/>
       <c r="B235" s="17" t="s">
         <v>2292</v>
@@ -42562,7 +42575,7 @@
       <c r="CT235" s="10"/>
       <c r="CU235" s="10"/>
     </row>
-    <row r="236" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:99">
       <c r="A236" s="108"/>
       <c r="B236" s="10"/>
       <c r="C236" s="10"/>
@@ -42663,7 +42676,7 @@
       <c r="CT236" s="10"/>
       <c r="CU236" s="10"/>
     </row>
-    <row r="237" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:99">
       <c r="A237" s="108"/>
       <c r="B237" s="17" t="s">
         <v>2336</v>
@@ -42804,7 +42817,7 @@
       <c r="CT237" s="10"/>
       <c r="CU237" s="10"/>
     </row>
-    <row r="238" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:99">
       <c r="A238" s="108"/>
       <c r="B238" s="10"/>
       <c r="C238" s="10"/>
@@ -42905,7 +42918,7 @@
       <c r="CT238" s="10"/>
       <c r="CU238" s="10"/>
     </row>
-    <row r="239" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:99">
       <c r="A239" s="108"/>
       <c r="B239" s="17" t="s">
         <v>2356</v>
@@ -43026,7 +43039,7 @@
       <c r="CT239" s="10"/>
       <c r="CU239" s="10"/>
     </row>
-    <row r="240" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:99">
       <c r="A240" s="108"/>
       <c r="B240" s="10"/>
       <c r="C240" s="10"/>
@@ -43127,7 +43140,7 @@
       <c r="CT240" s="10"/>
       <c r="CU240" s="10"/>
     </row>
-    <row r="241" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:99">
       <c r="A241" s="108"/>
       <c r="B241" s="17" t="s">
         <v>2366</v>
@@ -43262,7 +43275,7 @@
       <c r="CT241" s="10"/>
       <c r="CU241" s="10"/>
     </row>
-    <row r="242" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:99">
       <c r="A242" s="108"/>
       <c r="B242" s="10"/>
       <c r="C242" s="10"/>
@@ -43363,7 +43376,7 @@
       <c r="CT242" s="10"/>
       <c r="CU242" s="10"/>
     </row>
-    <row r="243" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:99">
       <c r="A243" s="108"/>
       <c r="B243" s="17" t="s">
         <v>2383</v>
@@ -43500,7 +43513,7 @@
       <c r="CT243" s="10"/>
       <c r="CU243" s="10"/>
     </row>
-    <row r="244" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:99">
       <c r="A244" s="108"/>
       <c r="B244" s="10"/>
       <c r="C244" s="10"/>
@@ -43601,7 +43614,7 @@
       <c r="CT244" s="10"/>
       <c r="CU244" s="10"/>
     </row>
-    <row r="245" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:99">
       <c r="A245" s="108"/>
       <c r="B245" s="17" t="s">
         <v>2401</v>
@@ -43732,7 +43745,7 @@
       <c r="CT245" s="10"/>
       <c r="CU245" s="10"/>
     </row>
-    <row r="246" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:99">
       <c r="A246" s="108"/>
       <c r="B246" s="10"/>
       <c r="C246" s="10"/>
@@ -43833,7 +43846,7 @@
       <c r="CT246" s="10"/>
       <c r="CU246" s="10"/>
     </row>
-    <row r="247" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:99">
       <c r="A247" s="108"/>
       <c r="B247" s="17" t="s">
         <v>2416</v>
@@ -43948,7 +43961,7 @@
       <c r="CT247" s="10"/>
       <c r="CU247" s="10"/>
     </row>
-    <row r="248" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:99">
       <c r="A248" s="108"/>
       <c r="B248" s="10"/>
       <c r="C248" s="10"/>
@@ -44049,7 +44062,7 @@
       <c r="CT248" s="10"/>
       <c r="CU248" s="10"/>
     </row>
-    <row r="249" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:99">
       <c r="A249" s="108"/>
       <c r="B249" s="17" t="s">
         <v>2423</v>
@@ -44220,7 +44233,7 @@
       <c r="CT249" s="10"/>
       <c r="CU249" s="10"/>
     </row>
-    <row r="250" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:99">
       <c r="A250" s="108"/>
       <c r="B250" s="10"/>
       <c r="C250" s="10"/>
@@ -44321,7 +44334,7 @@
       <c r="CT250" s="10"/>
       <c r="CU250" s="10"/>
     </row>
-    <row r="251" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:99">
       <c r="A251" s="10"/>
       <c r="B251" s="10" t="s">
         <v>242</v>
@@ -44502,7 +44515,7 @@
       <c r="CT251" s="10"/>
       <c r="CU251" s="10"/>
     </row>
-    <row r="252" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:99">
       <c r="A252" s="10"/>
       <c r="B252" s="10"/>
       <c r="C252" s="10"/>
@@ -44603,7 +44616,7 @@
       <c r="CT252" s="10"/>
       <c r="CU252" s="10"/>
     </row>
-    <row r="253" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:99">
       <c r="A253" s="10"/>
       <c r="B253" s="10"/>
       <c r="C253" s="10"/>
@@ -44704,7 +44717,7 @@
       <c r="CT253" s="10"/>
       <c r="CU253" s="10"/>
     </row>
-    <row r="254" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:99">
       <c r="A254" s="10"/>
       <c r="B254" s="10"/>
       <c r="C254" s="10"/>
@@ -44805,7 +44818,7 @@
       <c r="CT254" s="10"/>
       <c r="CU254" s="10"/>
     </row>
-    <row r="255" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:99">
       <c r="A255" s="10"/>
       <c r="B255" s="10"/>
       <c r="C255" s="10"/>
@@ -44906,7 +44919,7 @@
       <c r="CT255" s="10"/>
       <c r="CU255" s="10"/>
     </row>
-    <row r="256" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:99">
       <c r="A256" s="10"/>
       <c r="B256" s="10"/>
       <c r="C256" s="10"/>
@@ -45007,7 +45020,7 @@
       <c r="CT256" s="10"/>
       <c r="CU256" s="10"/>
     </row>
-    <row r="257" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:99">
       <c r="A257" s="10"/>
       <c r="B257" s="10"/>
       <c r="C257" s="10"/>
@@ -45108,7 +45121,7 @@
       <c r="CT257" s="10"/>
       <c r="CU257" s="10"/>
     </row>
-    <row r="258" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:99">
       <c r="A258" s="10"/>
       <c r="B258" s="10"/>
       <c r="C258" s="10"/>
@@ -45209,7 +45222,7 @@
       <c r="CT258" s="10"/>
       <c r="CU258" s="10"/>
     </row>
-    <row r="259" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:99">
       <c r="A259" s="10"/>
       <c r="B259" s="10"/>
       <c r="C259" s="10"/>
@@ -45310,7 +45323,7 @@
       <c r="CT259" s="10"/>
       <c r="CU259" s="10"/>
     </row>
-    <row r="260" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:99">
       <c r="A260" s="10"/>
       <c r="B260" s="10"/>
       <c r="C260" s="10"/>
@@ -45411,7 +45424,7 @@
       <c r="CT260" s="10"/>
       <c r="CU260" s="10"/>
     </row>
-    <row r="261" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:99">
       <c r="A261" s="10"/>
       <c r="B261" s="10"/>
       <c r="C261" s="10"/>
@@ -45512,7 +45525,7 @@
       <c r="CT261" s="10"/>
       <c r="CU261" s="10"/>
     </row>
-    <row r="262" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:99">
       <c r="A262" s="10"/>
       <c r="B262" s="10"/>
       <c r="C262" s="10"/>
@@ -45613,7 +45626,7 @@
       <c r="CT262" s="10"/>
       <c r="CU262" s="10"/>
     </row>
-    <row r="263" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:99">
       <c r="A263" s="10"/>
       <c r="B263" s="10"/>
       <c r="C263" s="10"/>
@@ -45714,7 +45727,7 @@
       <c r="CT263" s="10"/>
       <c r="CU263" s="10"/>
     </row>
-    <row r="264" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:99">
       <c r="A264" s="10"/>
       <c r="B264" s="10"/>
       <c r="C264" s="10"/>
@@ -45815,7 +45828,7 @@
       <c r="CT264" s="10"/>
       <c r="CU264" s="10"/>
     </row>
-    <row r="265" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:99">
       <c r="A265" s="10"/>
       <c r="B265" s="10"/>
       <c r="C265" s="10"/>
@@ -45916,7 +45929,7 @@
       <c r="CT265" s="10"/>
       <c r="CU265" s="10"/>
     </row>
-    <row r="266" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:99">
       <c r="A266" s="10"/>
       <c r="B266" s="10"/>
       <c r="C266" s="10"/>
@@ -46017,7 +46030,7 @@
       <c r="CT266" s="10"/>
       <c r="CU266" s="10"/>
     </row>
-    <row r="267" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:99">
       <c r="A267" s="10"/>
       <c r="B267" s="10"/>
       <c r="C267" s="10"/>
@@ -46118,7 +46131,7 @@
       <c r="CT267" s="10"/>
       <c r="CU267" s="10"/>
     </row>
-    <row r="268" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:99">
       <c r="A268" s="10"/>
       <c r="B268" s="10"/>
       <c r="C268" s="10"/>
@@ -46219,7 +46232,7 @@
       <c r="CT268" s="10"/>
       <c r="CU268" s="10"/>
     </row>
-    <row r="269" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:99">
       <c r="A269" s="10"/>
       <c r="B269" s="10"/>
       <c r="C269" s="10"/>
@@ -46320,7 +46333,7 @@
       <c r="CT269" s="10"/>
       <c r="CU269" s="10"/>
     </row>
-    <row r="270" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:99">
       <c r="A270" s="10"/>
       <c r="B270" s="10"/>
       <c r="C270" s="10"/>
@@ -46421,7 +46434,7 @@
       <c r="CT270" s="10"/>
       <c r="CU270" s="10"/>
     </row>
-    <row r="271" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:99">
       <c r="A271" s="10"/>
       <c r="B271" s="10"/>
       <c r="C271" s="10"/>
@@ -46522,7 +46535,7 @@
       <c r="CT271" s="10"/>
       <c r="CU271" s="10"/>
     </row>
-    <row r="272" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:99">
       <c r="A272" s="10"/>
       <c r="B272" s="10"/>
       <c r="C272" s="10"/>
@@ -46623,7 +46636,7 @@
       <c r="CT272" s="10"/>
       <c r="CU272" s="10"/>
     </row>
-    <row r="273" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:99">
       <c r="A273" s="10"/>
       <c r="B273" s="10"/>
       <c r="C273" s="10"/>
@@ -46724,7 +46737,7 @@
       <c r="CT273" s="10"/>
       <c r="CU273" s="10"/>
     </row>
-    <row r="274" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:99">
       <c r="A274" s="10"/>
       <c r="B274" s="10"/>
       <c r="C274" s="10"/>
@@ -46825,7 +46838,7 @@
       <c r="CT274" s="10"/>
       <c r="CU274" s="10"/>
     </row>
-    <row r="275" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:99">
       <c r="A275" s="10"/>
       <c r="B275" s="10"/>
       <c r="C275" s="10"/>
@@ -46926,7 +46939,7 @@
       <c r="CT275" s="10"/>
       <c r="CU275" s="10"/>
     </row>
-    <row r="276" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:99">
       <c r="A276" s="10"/>
       <c r="B276" s="10"/>
       <c r="C276" s="10"/>
@@ -47027,7 +47040,7 @@
       <c r="CT276" s="10"/>
       <c r="CU276" s="10"/>
     </row>
-    <row r="277" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:99">
       <c r="A277" s="10"/>
       <c r="B277" s="10"/>
       <c r="C277" s="10"/>
@@ -47128,7 +47141,7 @@
       <c r="CT277" s="10"/>
       <c r="CU277" s="10"/>
     </row>
-    <row r="278" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:99">
       <c r="A278" s="10"/>
       <c r="B278" s="10"/>
       <c r="C278" s="10"/>
@@ -47229,7 +47242,7 @@
       <c r="CT278" s="10"/>
       <c r="CU278" s="10"/>
     </row>
-    <row r="279" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:99">
       <c r="A279" s="10"/>
       <c r="B279" s="10"/>
       <c r="C279" s="10"/>
@@ -47330,7 +47343,7 @@
       <c r="CT279" s="10"/>
       <c r="CU279" s="10"/>
     </row>
-    <row r="280" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:99">
       <c r="A280" s="10"/>
       <c r="B280" s="10"/>
       <c r="C280" s="10"/>
@@ -47431,7 +47444,7 @@
       <c r="CT280" s="10"/>
       <c r="CU280" s="10"/>
     </row>
-    <row r="281" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:99">
       <c r="A281" s="10"/>
       <c r="B281" s="10"/>
       <c r="C281" s="10"/>
@@ -47532,7 +47545,7 @@
       <c r="CT281" s="10"/>
       <c r="CU281" s="10"/>
     </row>
-    <row r="282" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:99">
       <c r="A282" s="10"/>
       <c r="B282" s="10"/>
       <c r="C282" s="10"/>
@@ -47633,7 +47646,7 @@
       <c r="CT282" s="10"/>
       <c r="CU282" s="10"/>
     </row>
-    <row r="283" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:99">
       <c r="A283" s="10"/>
       <c r="B283" s="10"/>
       <c r="C283" s="10"/>
@@ -47734,7 +47747,7 @@
       <c r="CT283" s="10"/>
       <c r="CU283" s="10"/>
     </row>
-    <row r="284" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:99">
       <c r="A284" s="10"/>
       <c r="B284" s="10"/>
       <c r="C284" s="10"/>
@@ -47835,7 +47848,7 @@
       <c r="CT284" s="10"/>
       <c r="CU284" s="10"/>
     </row>
-    <row r="285" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:99">
       <c r="A285" s="10"/>
       <c r="B285" s="10"/>
       <c r="C285" s="10"/>
@@ -47936,7 +47949,7 @@
       <c r="CT285" s="10"/>
       <c r="CU285" s="10"/>
     </row>
-    <row r="286" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:99">
       <c r="A286" s="10"/>
       <c r="B286" s="10"/>
       <c r="C286" s="10"/>
@@ -48037,7 +48050,7 @@
       <c r="CT286" s="10"/>
       <c r="CU286" s="10"/>
     </row>
-    <row r="287" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:99">
       <c r="A287" s="10"/>
       <c r="B287" s="10"/>
       <c r="C287" s="10"/>
@@ -48138,7 +48151,7 @@
       <c r="CT287" s="10"/>
       <c r="CU287" s="10"/>
     </row>
-    <row r="288" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:99">
       <c r="A288" s="10"/>
       <c r="B288" s="10"/>
       <c r="C288" s="10"/>
@@ -48239,7 +48252,7 @@
       <c r="CT288" s="10"/>
       <c r="CU288" s="10"/>
     </row>
-    <row r="289" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:99">
       <c r="A289" s="10"/>
       <c r="B289" s="10"/>
       <c r="C289" s="10"/>
@@ -48340,7 +48353,7 @@
       <c r="CT289" s="10"/>
       <c r="CU289" s="10"/>
     </row>
-    <row r="290" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:99">
       <c r="A290" s="10"/>
       <c r="B290" s="10"/>
       <c r="C290" s="10"/>
@@ -48441,7 +48454,7 @@
       <c r="CT290" s="10"/>
       <c r="CU290" s="10"/>
     </row>
-    <row r="291" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:99">
       <c r="A291" s="10"/>
       <c r="B291" s="10"/>
       <c r="C291" s="10"/>
@@ -48542,7 +48555,7 @@
       <c r="CT291" s="10"/>
       <c r="CU291" s="10"/>
     </row>
-    <row r="292" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:99">
       <c r="A292" s="10"/>
       <c r="B292" s="10"/>
       <c r="C292" s="10"/>
@@ -48643,7 +48656,7 @@
       <c r="CT292" s="10"/>
       <c r="CU292" s="10"/>
     </row>
-    <row r="293" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:99">
       <c r="A293" s="10"/>
       <c r="B293" s="10"/>
       <c r="C293" s="10"/>
@@ -48744,7 +48757,7 @@
       <c r="CT293" s="10"/>
       <c r="CU293" s="10"/>
     </row>
-    <row r="294" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:99">
       <c r="A294" s="10"/>
       <c r="B294" s="10"/>
       <c r="C294" s="10"/>
@@ -48845,7 +48858,7 @@
       <c r="CT294" s="10"/>
       <c r="CU294" s="10"/>
     </row>
-    <row r="295" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:99">
       <c r="A295" s="10"/>
       <c r="B295" s="10"/>
       <c r="C295" s="10"/>
@@ -48946,7 +48959,7 @@
       <c r="CT295" s="10"/>
       <c r="CU295" s="10"/>
     </row>
-    <row r="296" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:99">
       <c r="A296" s="10"/>
       <c r="B296" s="10"/>
       <c r="C296" s="10"/>
@@ -49047,7 +49060,7 @@
       <c r="CT296" s="10"/>
       <c r="CU296" s="10"/>
     </row>
-    <row r="297" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:99">
       <c r="A297" s="10"/>
       <c r="B297" s="10"/>
       <c r="C297" s="10"/>
@@ -49148,7 +49161,7 @@
       <c r="CT297" s="10"/>
       <c r="CU297" s="10"/>
     </row>
-    <row r="298" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:99">
       <c r="A298" s="10"/>
       <c r="B298" s="10"/>
       <c r="C298" s="10"/>
@@ -49249,7 +49262,7 @@
       <c r="CT298" s="10"/>
       <c r="CU298" s="10"/>
     </row>
-    <row r="299" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:99">
       <c r="A299" s="10"/>
       <c r="B299" s="10"/>
       <c r="C299" s="10"/>
@@ -49350,7 +49363,7 @@
       <c r="CT299" s="10"/>
       <c r="CU299" s="10"/>
     </row>
-    <row r="300" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:99">
       <c r="A300" s="10"/>
       <c r="B300" s="10"/>
       <c r="C300" s="10"/>
@@ -49451,7 +49464,7 @@
       <c r="CT300" s="10"/>
       <c r="CU300" s="10"/>
     </row>
-    <row r="301" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:99">
       <c r="A301" s="10"/>
       <c r="B301" s="10"/>
       <c r="C301" s="10"/>
@@ -49552,7 +49565,7 @@
       <c r="CT301" s="10"/>
       <c r="CU301" s="10"/>
     </row>
-    <row r="302" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:99">
       <c r="A302" s="10"/>
       <c r="B302" s="10"/>
       <c r="C302" s="10"/>
@@ -49653,7 +49666,7 @@
       <c r="CT302" s="10"/>
       <c r="CU302" s="10"/>
     </row>
-    <row r="303" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:99">
       <c r="A303" s="10"/>
       <c r="B303" s="10"/>
       <c r="C303" s="10"/>
@@ -49754,7 +49767,7 @@
       <c r="CT303" s="10"/>
       <c r="CU303" s="10"/>
     </row>
-    <row r="304" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:99">
       <c r="A304" s="10"/>
       <c r="B304" s="10"/>
       <c r="C304" s="10"/>
@@ -49855,7 +49868,7 @@
       <c r="CT304" s="10"/>
       <c r="CU304" s="10"/>
     </row>
-    <row r="305" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:99">
       <c r="A305" s="10"/>
       <c r="B305" s="10"/>
       <c r="C305" s="10"/>
@@ -49956,7 +49969,7 @@
       <c r="CT305" s="10"/>
       <c r="CU305" s="10"/>
     </row>
-    <row r="306" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:99">
       <c r="A306" s="10"/>
       <c r="B306" s="10"/>
       <c r="C306" s="10"/>
@@ -50057,7 +50070,7 @@
       <c r="CT306" s="10"/>
       <c r="CU306" s="10"/>
     </row>
-    <row r="307" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:99">
       <c r="A307" s="10"/>
       <c r="B307" s="10"/>
       <c r="C307" s="10"/>
@@ -50158,7 +50171,7 @@
       <c r="CT307" s="10"/>
       <c r="CU307" s="10"/>
     </row>
-    <row r="308" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:99">
       <c r="A308" s="10"/>
       <c r="B308" s="10"/>
       <c r="C308" s="10"/>
@@ -50259,7 +50272,7 @@
       <c r="CT308" s="10"/>
       <c r="CU308" s="10"/>
     </row>
-    <row r="309" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:99">
       <c r="A309" s="10"/>
       <c r="B309" s="10"/>
       <c r="C309" s="10"/>
@@ -50360,7 +50373,7 @@
       <c r="CT309" s="10"/>
       <c r="CU309" s="10"/>
     </row>
-    <row r="310" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:99">
       <c r="A310" s="10"/>
       <c r="B310" s="10"/>
       <c r="C310" s="10"/>
@@ -50461,7 +50474,7 @@
       <c r="CT310" s="10"/>
       <c r="CU310" s="10"/>
     </row>
-    <row r="311" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:99">
       <c r="A311" s="10"/>
       <c r="B311" s="10"/>
       <c r="C311" s="10"/>
@@ -50562,7 +50575,7 @@
       <c r="CT311" s="10"/>
       <c r="CU311" s="10"/>
     </row>
-    <row r="312" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:99">
       <c r="A312" s="10"/>
       <c r="B312" s="10"/>
       <c r="C312" s="10"/>
@@ -50663,7 +50676,7 @@
       <c r="CT312" s="10"/>
       <c r="CU312" s="10"/>
     </row>
-    <row r="313" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:99">
       <c r="A313" s="10"/>
       <c r="B313" s="10"/>
       <c r="C313" s="10"/>
@@ -50764,7 +50777,7 @@
       <c r="CT313" s="10"/>
       <c r="CU313" s="10"/>
     </row>
-    <row r="314" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:99">
       <c r="A314" s="10"/>
       <c r="B314" s="10"/>
       <c r="C314" s="10"/>
@@ -50865,7 +50878,7 @@
       <c r="CT314" s="10"/>
       <c r="CU314" s="10"/>
     </row>
-    <row r="315" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:99">
       <c r="A315" s="10"/>
       <c r="B315" s="10"/>
       <c r="C315" s="10"/>
@@ -50966,7 +50979,7 @@
       <c r="CT315" s="10"/>
       <c r="CU315" s="10"/>
     </row>
-    <row r="316" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:99">
       <c r="A316" s="10"/>
       <c r="B316" s="10"/>
       <c r="C316" s="10"/>
@@ -51067,7 +51080,7 @@
       <c r="CT316" s="10"/>
       <c r="CU316" s="10"/>
     </row>
-    <row r="317" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:99">
       <c r="A317" s="10"/>
       <c r="B317" s="10"/>
       <c r="C317" s="10"/>
@@ -51168,7 +51181,7 @@
       <c r="CT317" s="10"/>
       <c r="CU317" s="10"/>
     </row>
-    <row r="318" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:99">
       <c r="A318" s="10"/>
       <c r="B318" s="10"/>
       <c r="C318" s="10"/>
@@ -51269,7 +51282,7 @@
       <c r="CT318" s="10"/>
       <c r="CU318" s="10"/>
     </row>
-    <row r="319" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:99">
       <c r="A319" s="10"/>
       <c r="B319" s="10"/>
       <c r="C319" s="10"/>
@@ -51370,7 +51383,7 @@
       <c r="CT319" s="10"/>
       <c r="CU319" s="10"/>
     </row>
-    <row r="320" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:99">
       <c r="A320" s="10"/>
       <c r="B320" s="10"/>
       <c r="C320" s="10"/>
@@ -51471,7 +51484,7 @@
       <c r="CT320" s="10"/>
       <c r="CU320" s="10"/>
     </row>
-    <row r="321" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="321" spans="2:81">
       <c r="B321" s="10"/>
       <c r="C321" s="10"/>
       <c r="D321" s="10"/>
@@ -51553,7 +51566,7 @@
       <c r="CB321" s="10"/>
       <c r="CC321" s="10"/>
     </row>
-    <row r="322" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="322" spans="2:81">
       <c r="B322" s="10"/>
       <c r="C322" s="10"/>
       <c r="D322" s="10"/>
@@ -51635,7 +51648,7 @@
       <c r="CB322" s="10"/>
       <c r="CC322" s="10"/>
     </row>
-    <row r="323" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="323" spans="2:81">
       <c r="B323" s="10"/>
       <c r="C323" s="10"/>
       <c r="D323" s="10"/>
@@ -51717,7 +51730,7 @@
       <c r="CB323" s="10"/>
       <c r="CC323" s="10"/>
     </row>
-    <row r="324" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="324" spans="2:81">
       <c r="B324" s="10"/>
       <c r="C324" s="10"/>
       <c r="D324" s="10"/>
@@ -51817,13 +51830,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1"/>
       <c r="B1" s="109" t="s">
         <v>0</v>
@@ -51855,7 +51868,7 @@
       <c r="W1" s="109"/>
       <c r="X1" s="109"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>2595</v>
@@ -51923,7 +51936,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" s="4" t="s">
         <v>2625</v>
       </c>
@@ -51959,7 +51972,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" s="5" t="s">
         <v>2596</v>
       </c>
@@ -51991,7 +52004,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -52021,7 +52034,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" s="4" t="s">
         <v>2644</v>
       </c>
@@ -52057,7 +52070,7 @@
       </c>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -52087,7 +52100,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -52117,7 +52130,7 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24">
       <c r="A9" s="5" t="s">
         <v>2531</v>
       </c>
@@ -52149,7 +52162,7 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24">
       <c r="A10" s="4" t="s">
         <v>2648</v>
       </c>
@@ -52185,7 +52198,7 @@
       <c r="W10" s="6"/>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24">
       <c r="A11" s="5" t="s">
         <v>2468</v>
       </c>
@@ -52215,7 +52228,7 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24">
       <c r="A12" s="5" t="s">
         <v>2497</v>
       </c>
@@ -52245,7 +52258,7 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -52274,7 +52287,7 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -52303,7 +52316,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -52333,7 +52346,7 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -52355,14 +52368,16 @@
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
+      <c r="S16" s="110" t="s">
+        <v>2813</v>
+      </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:57">
       <c r="A17" s="5" t="s">
         <v>2514</v>
       </c>
@@ -52394,7 +52409,7 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:57">
       <c r="A18" s="4" t="s">
         <v>2543</v>
       </c>
@@ -52428,7 +52443,7 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:57">
       <c r="A19" s="4" t="s">
         <v>2541</v>
       </c>
@@ -52462,7 +52477,7 @@
         <v>2539</v>
       </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:57">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -52492,7 +52507,7 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:57">
       <c r="A21" s="4" t="s">
         <v>2536</v>
       </c>
@@ -52528,7 +52543,7 @@
         <v>2471</v>
       </c>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:57">
       <c r="A22" s="5" t="s">
         <v>2636</v>
       </c>
@@ -52564,7 +52579,7 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:57">
       <c r="A23" s="4" t="s">
         <v>2642</v>
       </c>
@@ -52600,7 +52615,7 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:57">
       <c r="A24" s="5" t="s">
         <v>2520</v>
       </c>
@@ -52632,7 +52647,7 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:57">
       <c r="A25" s="5" t="s">
         <v>2525</v>
       </c>
@@ -52664,7 +52679,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:57">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
@@ -52694,7 +52709,7 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:57">
       <c r="A27" s="5" t="s">
         <v>2508</v>
       </c>
@@ -52726,7 +52741,7 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:57">
       <c r="A28" s="5" t="s">
         <v>2528</v>
       </c>
@@ -52758,7 +52773,7 @@
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:57">
       <c r="A29" s="5" t="s">
         <v>2466</v>
       </c>
@@ -52791,12 +52806,12 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:57">
       <c r="AY30" t="s">
         <v>2621</v>
       </c>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:57">
       <c r="AW31" t="s">
         <v>2478</v>
       </c>
@@ -52807,7 +52822,7 @@
         <v>2616</v>
       </c>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:57">
       <c r="A32" s="1"/>
       <c r="B32" s="11" t="s">
         <v>16</v>
@@ -52978,7 +52993,7 @@
         <v>2615</v>
       </c>
     </row>
-    <row r="33" spans="1:59" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:59" ht="409.5">
       <c r="A33" s="12" t="s">
         <v>71</v>
       </c>
@@ -53153,7 +53168,7 @@
       <c r="BF33" s="31"/>
       <c r="BG33" s="31"/>
     </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:59">
       <c r="AL34" t="s">
         <v>2573</v>
       </c>
@@ -53161,7 +53176,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:59">
       <c r="A37" s="29"/>
       <c r="B37" s="109" t="s">
         <v>0</v>
@@ -53193,7 +53208,7 @@
       <c r="W37" s="109"/>
       <c r="X37" s="109"/>
     </row>
-    <row r="38" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:59">
       <c r="A38" s="28"/>
       <c r="B38" s="4" t="s">
         <v>2595</v>
@@ -53261,7 +53276,7 @@
         <v>2589</v>
       </c>
     </row>
-    <row r="39" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:59">
       <c r="A39" s="4" t="s">
         <v>2586</v>
       </c>
@@ -53295,7 +53310,7 @@
       <c r="W39" s="28"/>
       <c r="X39" s="28"/>
     </row>
-    <row r="40" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:59">
       <c r="A40" s="5" t="s">
         <v>2596</v>
       </c>
@@ -53327,7 +53342,7 @@
       <c r="W40" s="28"/>
       <c r="X40" s="28"/>
     </row>
-    <row r="41" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:59">
       <c r="A41" s="5" t="s">
         <v>4</v>
       </c>
@@ -53357,7 +53372,7 @@
       <c r="W41" s="28"/>
       <c r="X41" s="28"/>
     </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:59">
       <c r="A42" s="4" t="s">
         <v>2606</v>
       </c>
@@ -53389,7 +53404,7 @@
       <c r="W42" s="28"/>
       <c r="X42" s="28"/>
     </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:59">
       <c r="A43" s="5" t="s">
         <v>6</v>
       </c>
@@ -53419,7 +53434,7 @@
       <c r="W43" s="28"/>
       <c r="X43" s="28"/>
     </row>
-    <row r="44" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:59">
       <c r="A44" s="5" t="s">
         <v>8</v>
       </c>
@@ -53449,7 +53464,7 @@
       <c r="W44" s="28"/>
       <c r="X44" s="28"/>
     </row>
-    <row r="45" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:59">
       <c r="A45" s="5" t="s">
         <v>2582</v>
       </c>
@@ -53481,7 +53496,7 @@
       <c r="W45" s="28"/>
       <c r="X45" s="28"/>
     </row>
-    <row r="46" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:59">
       <c r="A46" s="4" t="s">
         <v>2602</v>
       </c>
@@ -53513,7 +53528,7 @@
       <c r="W46" s="6"/>
       <c r="X46" s="28"/>
     </row>
-    <row r="47" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:59">
       <c r="A47" s="5" t="s">
         <v>2468</v>
       </c>
@@ -53543,7 +53558,7 @@
       <c r="W47" s="28"/>
       <c r="X47" s="28"/>
     </row>
-    <row r="48" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:59">
       <c r="A48" s="5" t="s">
         <v>2547</v>
       </c>
@@ -53573,7 +53588,7 @@
       <c r="W48" s="28"/>
       <c r="X48" s="28"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24">
       <c r="A49" s="5" t="s">
         <v>10</v>
       </c>
@@ -53603,7 +53618,7 @@
       <c r="W49" s="28"/>
       <c r="X49" s="28"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24">
       <c r="A50" s="5" t="s">
         <v>12</v>
       </c>
@@ -53632,7 +53647,7 @@
       <c r="W50" s="28"/>
       <c r="X50" s="28"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24">
       <c r="A51" s="5" t="s">
         <v>14</v>
       </c>
@@ -53662,7 +53677,7 @@
       <c r="W51" s="28"/>
       <c r="X51" s="28"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24">
       <c r="A52" s="5" t="s">
         <v>16</v>
       </c>
@@ -53691,7 +53706,7 @@
       <c r="W52" s="28"/>
       <c r="X52" s="28"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24">
       <c r="A53" s="5" t="s">
         <v>2514</v>
       </c>
@@ -53723,7 +53738,7 @@
       <c r="W53" s="28"/>
       <c r="X53" s="28"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24">
       <c r="A54" s="4" t="s">
         <v>2543</v>
       </c>
@@ -53757,7 +53772,7 @@
       <c r="W54" s="28"/>
       <c r="X54" s="28"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24">
       <c r="A55" s="4" t="s">
         <v>2541</v>
       </c>
@@ -53791,7 +53806,7 @@
         <v>2588</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24">
       <c r="A56" s="5" t="s">
         <v>20</v>
       </c>
@@ -53821,7 +53836,7 @@
       <c r="W56" s="28"/>
       <c r="X56" s="28"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24">
       <c r="A57" s="4" t="s">
         <v>2584</v>
       </c>
@@ -53855,7 +53870,7 @@
         <v>2471</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24">
       <c r="A58" s="5" t="s">
         <v>2562</v>
       </c>
@@ -53889,7 +53904,7 @@
       <c r="W58" s="28"/>
       <c r="X58" s="28"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24">
       <c r="A59" s="4" t="s">
         <v>2599</v>
       </c>
@@ -53923,7 +53938,7 @@
       <c r="W59" s="28"/>
       <c r="X59" s="28"/>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24">
       <c r="A60" s="5" t="s">
         <v>2520</v>
       </c>
@@ -53955,7 +53970,7 @@
       <c r="W60" s="28"/>
       <c r="X60" s="28"/>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24">
       <c r="A61" s="5" t="s">
         <v>2577</v>
       </c>
@@ -53987,7 +54002,7 @@
       <c r="W61" s="28"/>
       <c r="X61" s="28"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24">
       <c r="A62" s="5" t="s">
         <v>22</v>
       </c>
@@ -54017,7 +54032,7 @@
       <c r="W62" s="28"/>
       <c r="X62" s="28"/>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24">
       <c r="A63" s="5" t="s">
         <v>2566</v>
       </c>
@@ -54049,7 +54064,7 @@
       <c r="W63" s="28"/>
       <c r="X63" s="28"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24">
       <c r="A64" s="5" t="s">
         <v>2528</v>
       </c>
@@ -54081,7 +54096,7 @@
       <c r="W64" s="28"/>
       <c r="X64" s="28"/>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24">
       <c r="A65" s="5" t="s">
         <v>2466</v>
       </c>
@@ -54137,12 +54152,12 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="22" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18" thickBot="1">
       <c r="A1" s="84"/>
       <c r="B1" s="85" t="s">
         <v>2681</v>
@@ -54208,7 +54223,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="18" thickTop="1">
       <c r="A2" s="92" t="s">
         <v>2654</v>
       </c>
@@ -54240,7 +54255,7 @@
         <v>2748</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="17.25">
       <c r="A3" s="93" t="s">
         <v>2655</v>
       </c>
@@ -54272,7 +54287,7 @@
       <c r="U3" s="48"/>
       <c r="V3" s="49"/>
     </row>
-    <row r="4" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="17.25">
       <c r="A4" s="93" t="s">
         <v>2657</v>
       </c>
@@ -54304,7 +54319,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="17.25">
       <c r="A5" s="93" t="s">
         <v>2660</v>
       </c>
@@ -54336,7 +54351,7 @@
       <c r="U5" s="48"/>
       <c r="V5" s="49"/>
     </row>
-    <row r="6" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="17.25">
       <c r="A6" s="93" t="s">
         <v>2702</v>
       </c>
@@ -54368,7 +54383,7 @@
       <c r="U6" s="48"/>
       <c r="V6" s="49"/>
     </row>
-    <row r="7" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="17.25">
       <c r="A7" s="93" t="s">
         <v>2703</v>
       </c>
@@ -54400,7 +54415,7 @@
       <c r="U7" s="48"/>
       <c r="V7" s="49"/>
     </row>
-    <row r="8" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="17.25">
       <c r="A8" s="93" t="s">
         <v>2669</v>
       </c>
@@ -54432,7 +54447,7 @@
       <c r="U8" s="48"/>
       <c r="V8" s="49"/>
     </row>
-    <row r="9" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="17.25">
       <c r="A9" s="93" t="s">
         <v>2670</v>
       </c>
@@ -54464,7 +54479,7 @@
       <c r="U9" s="55"/>
       <c r="V9" s="49"/>
     </row>
-    <row r="10" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="17.25">
       <c r="A10" s="93" t="s">
         <v>2704</v>
       </c>
@@ -54496,7 +54511,7 @@
       <c r="U10" s="48"/>
       <c r="V10" s="49"/>
     </row>
-    <row r="11" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="17.25">
       <c r="A11" s="93" t="s">
         <v>2705</v>
       </c>
@@ -54528,7 +54543,7 @@
       <c r="U11" s="48"/>
       <c r="V11" s="49"/>
     </row>
-    <row r="12" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="17.25">
       <c r="A12" s="93" t="s">
         <v>2673</v>
       </c>
@@ -54560,7 +54575,7 @@
       <c r="U12" s="48"/>
       <c r="V12" s="49"/>
     </row>
-    <row r="13" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="17.25">
       <c r="A13" s="93" t="s">
         <v>2706</v>
       </c>
@@ -54592,7 +54607,7 @@
       <c r="U13" s="48"/>
       <c r="V13" s="49"/>
     </row>
-    <row r="14" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="17.25">
       <c r="A14" s="93" t="s">
         <v>2707</v>
       </c>
@@ -54624,7 +54639,7 @@
       <c r="U14" s="48"/>
       <c r="V14" s="49"/>
     </row>
-    <row r="15" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="17.25">
       <c r="A15" s="93" t="s">
         <v>2708</v>
       </c>
@@ -54656,7 +54671,7 @@
       </c>
       <c r="V15" s="49"/>
     </row>
-    <row r="16" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="17.25">
       <c r="A16" s="93" t="s">
         <v>2676</v>
       </c>
@@ -54688,7 +54703,7 @@
       </c>
       <c r="V16" s="49"/>
     </row>
-    <row r="17" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="17.25">
       <c r="A17" s="93" t="s">
         <v>2677</v>
       </c>
@@ -54720,7 +54735,7 @@
       <c r="U17" s="48"/>
       <c r="V17" s="49"/>
     </row>
-    <row r="18" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="17.25">
       <c r="A18" s="93" t="s">
         <v>2709</v>
       </c>
@@ -54752,7 +54767,7 @@
       <c r="U18" s="48"/>
       <c r="V18" s="49"/>
     </row>
-    <row r="19" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="17.25">
       <c r="A19" s="93" t="s">
         <v>2679</v>
       </c>
@@ -54784,7 +54799,7 @@
       <c r="U19" s="48"/>
       <c r="V19" s="49"/>
     </row>
-    <row r="20" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" ht="18" thickBot="1">
       <c r="A20" s="94" t="s">
         <v>2680</v>
       </c>
@@ -54816,7 +54831,7 @@
       <c r="U20" s="91"/>
       <c r="V20" s="65"/>
     </row>
-    <row r="21" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="17.25">
       <c r="A21" s="77"/>
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
@@ -54840,7 +54855,7 @@
       <c r="U21" s="79"/>
       <c r="V21" s="79"/>
     </row>
-    <row r="22" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="17.25">
       <c r="A22" s="77"/>
       <c r="B22" s="78"/>
       <c r="C22" s="78"/>
@@ -54864,7 +54879,7 @@
       <c r="U22" s="79"/>
       <c r="V22" s="79"/>
     </row>
-    <row r="23" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="17.25">
       <c r="A23" s="77"/>
       <c r="B23" s="78"/>
       <c r="C23" s="78"/>
@@ -54888,7 +54903,7 @@
       <c r="U23" s="79"/>
       <c r="V23" s="79"/>
     </row>
-    <row r="24" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="17.25">
       <c r="A24" s="77"/>
       <c r="B24" s="78"/>
       <c r="C24" s="78"/>
@@ -54912,7 +54927,7 @@
       <c r="U24" s="79"/>
       <c r="V24" s="79"/>
     </row>
-    <row r="25" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="17.25">
       <c r="A25" s="77"/>
       <c r="B25" s="78"/>
       <c r="C25" s="78"/>
@@ -54936,7 +54951,7 @@
       <c r="U25" s="79"/>
       <c r="V25" s="79"/>
     </row>
-    <row r="26" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="17.25">
       <c r="A26" s="77"/>
       <c r="B26" s="78"/>
       <c r="C26" s="78"/>
@@ -54960,7 +54975,7 @@
       <c r="U26" s="79"/>
       <c r="V26" s="79"/>
     </row>
-    <row r="27" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="17.25">
       <c r="A27" s="77"/>
       <c r="B27" s="78"/>
       <c r="C27" s="78"/>
@@ -54984,7 +54999,7 @@
       <c r="U27" s="79"/>
       <c r="V27" s="79"/>
     </row>
-    <row r="28" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="17.25">
       <c r="A28" s="77"/>
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
@@ -55026,12 +55041,12 @@
       <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="22" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18" thickBot="1">
       <c r="A1" s="70"/>
       <c r="B1" s="71" t="s">
         <v>2681</v>
@@ -55097,7 +55112,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="18" thickTop="1">
       <c r="A2" s="82" t="s">
         <v>2654</v>
       </c>
@@ -55131,7 +55146,7 @@
       <c r="U2" s="41"/>
       <c r="V2" s="43"/>
     </row>
-    <row r="3" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="17.25">
       <c r="A3" s="83" t="s">
         <v>2655</v>
       </c>
@@ -55161,7 +55176,7 @@
       <c r="U3" s="48"/>
       <c r="V3" s="49"/>
     </row>
-    <row r="4" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="17.25">
       <c r="A4" s="83" t="s">
         <v>2656</v>
       </c>
@@ -55189,7 +55204,7 @@
       <c r="U4" s="48"/>
       <c r="V4" s="49"/>
     </row>
-    <row r="5" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="17.25">
       <c r="A5" s="83" t="s">
         <v>2657</v>
       </c>
@@ -55223,7 +55238,7 @@
       </c>
       <c r="V5" s="49"/>
     </row>
-    <row r="6" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="17.25">
       <c r="A6" s="83" t="s">
         <v>2658</v>
       </c>
@@ -55251,7 +55266,7 @@
       <c r="U6" s="48"/>
       <c r="V6" s="49"/>
     </row>
-    <row r="7" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="17.25">
       <c r="A7" s="83" t="s">
         <v>2659</v>
       </c>
@@ -55279,7 +55294,7 @@
       <c r="U7" s="48"/>
       <c r="V7" s="49"/>
     </row>
-    <row r="8" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="17.25">
       <c r="A8" s="83" t="s">
         <v>2660</v>
       </c>
@@ -55309,7 +55324,7 @@
       <c r="U8" s="48"/>
       <c r="V8" s="49"/>
     </row>
-    <row r="9" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="17.25">
       <c r="A9" s="83" t="s">
         <v>2661</v>
       </c>
@@ -55343,7 +55358,7 @@
       <c r="U9" s="55"/>
       <c r="V9" s="49"/>
     </row>
-    <row r="10" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="17.25">
       <c r="A10" s="83" t="s">
         <v>2662</v>
       </c>
@@ -55371,7 +55386,7 @@
       <c r="U10" s="48"/>
       <c r="V10" s="49"/>
     </row>
-    <row r="11" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="17.25">
       <c r="A11" s="83" t="s">
         <v>2663</v>
       </c>
@@ -55399,7 +55414,7 @@
       <c r="U11" s="48"/>
       <c r="V11" s="49"/>
     </row>
-    <row r="12" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="17.25">
       <c r="A12" s="83" t="s">
         <v>2664</v>
       </c>
@@ -55427,7 +55442,7 @@
       <c r="U12" s="48"/>
       <c r="V12" s="49"/>
     </row>
-    <row r="13" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="17.25">
       <c r="A13" s="83" t="s">
         <v>2665</v>
       </c>
@@ -55455,7 +55470,7 @@
       <c r="U13" s="48"/>
       <c r="V13" s="49"/>
     </row>
-    <row r="14" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="17.25">
       <c r="A14" s="83" t="s">
         <v>2666</v>
       </c>
@@ -55483,7 +55498,7 @@
       <c r="U14" s="48"/>
       <c r="V14" s="49"/>
     </row>
-    <row r="15" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="17.25">
       <c r="A15" s="83" t="s">
         <v>2667</v>
       </c>
@@ -55511,7 +55526,7 @@
       <c r="U15" s="48"/>
       <c r="V15" s="49"/>
     </row>
-    <row r="16" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="17.25">
       <c r="A16" s="83" t="s">
         <v>2668</v>
       </c>
@@ -55541,7 +55556,7 @@
       <c r="U16" s="48"/>
       <c r="V16" s="49"/>
     </row>
-    <row r="17" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="17.25">
       <c r="A17" s="83" t="s">
         <v>2669</v>
       </c>
@@ -55573,7 +55588,7 @@
       <c r="U17" s="48"/>
       <c r="V17" s="49"/>
     </row>
-    <row r="18" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="17.25">
       <c r="A18" s="83" t="s">
         <v>2670</v>
       </c>
@@ -55605,7 +55620,7 @@
         <v>2539</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="17.25">
       <c r="A19" s="83" t="s">
         <v>2671</v>
       </c>
@@ -55633,7 +55648,7 @@
       <c r="U19" s="48"/>
       <c r="V19" s="49"/>
     </row>
-    <row r="20" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="17.25">
       <c r="A20" s="83" t="s">
         <v>2672</v>
       </c>
@@ -55667,7 +55682,7 @@
         <v>2471</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="17.25">
       <c r="A21" s="83" t="s">
         <v>2673</v>
       </c>
@@ -55701,7 +55716,7 @@
       <c r="U21" s="48"/>
       <c r="V21" s="49"/>
     </row>
-    <row r="22" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="17.25">
       <c r="A22" s="83" t="s">
         <v>2674</v>
       </c>
@@ -55735,7 +55750,7 @@
       <c r="U22" s="48"/>
       <c r="V22" s="49"/>
     </row>
-    <row r="23" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="17.25">
       <c r="A23" s="83" t="s">
         <v>2675</v>
       </c>
@@ -55765,7 +55780,7 @@
       <c r="U23" s="48"/>
       <c r="V23" s="49"/>
     </row>
-    <row r="24" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="17.25">
       <c r="A24" s="83" t="s">
         <v>2676</v>
       </c>
@@ -55795,7 +55810,7 @@
       <c r="U24" s="48"/>
       <c r="V24" s="49"/>
     </row>
-    <row r="25" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="17.25">
       <c r="A25" s="83" t="s">
         <v>2677</v>
       </c>
@@ -55823,7 +55838,7 @@
       <c r="U25" s="48"/>
       <c r="V25" s="49"/>
     </row>
-    <row r="26" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="17.25">
       <c r="A26" s="83" t="s">
         <v>2678</v>
       </c>
@@ -55853,7 +55868,7 @@
       <c r="U26" s="48"/>
       <c r="V26" s="49"/>
     </row>
-    <row r="27" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="17.25">
       <c r="A27" s="83" t="s">
         <v>2679</v>
       </c>
@@ -55883,7 +55898,7 @@
       <c r="U27" s="48"/>
       <c r="V27" s="49"/>
     </row>
-    <row r="28" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" ht="18" thickBot="1">
       <c r="A28" s="95" t="s">
         <v>2680</v>
       </c>
@@ -55929,12 +55944,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="19" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="103" t="s">
         <v>2807</v>
       </c>
@@ -55993,7 +56008,7 @@
         <v>2680</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="18" customHeight="1" thickTop="1">
       <c r="A2" s="100" t="s">
         <v>2710</v>
       </c>
@@ -56052,7 +56067,7 @@
         <v>2728</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="18" customHeight="1">
       <c r="A3" s="34" t="s">
         <v>2729</v>
       </c>
@@ -56111,7 +56126,7 @@
         <v>2785</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="18" customHeight="1">
       <c r="A4" s="34" t="s">
         <v>2786</v>
       </c>
@@ -56170,7 +56185,7 @@
         <v>2766</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="18" customHeight="1">
       <c r="A5" s="34" t="s">
         <v>2795</v>
       </c>
@@ -56229,7 +56244,7 @@
         <v>2479</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="18" customHeight="1">
       <c r="A6" s="34" t="s">
         <v>2517</v>
       </c>
@@ -56288,7 +56303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="18" customHeight="1" thickBot="1">
       <c r="A7" s="96" t="s">
         <v>2802</v>
       </c>

</xml_diff>